<commit_message>
* xlsx中Prop的撬开的缝隙isUnique属性改为No * 为stage增加interactiveprops组件，然后对stage使用道具为use interactive props
</commit_message>
<xml_diff>
--- a/budding_world/settings_editor/budding_world.xlsx
+++ b/budding_world/settings_editor/budding_world.xlsx
@@ -7,11 +7,11 @@
     <workbookView windowHeight="15800" windowWidth="28040" xWindow="4240" yWindow="640"/>
   </bookViews>
   <sheets>
-    <sheet name="封面说明" sheetId="2" r:id="rId5"/>
-    <sheet name="World2" sheetId="3" r:id="rId6"/>
-    <sheet name="Stage" sheetId="4" r:id="rId7"/>
-    <sheet name="NPC" sheetId="5" r:id="rId8"/>
-    <sheet name="Prop" sheetId="6" r:id="rId9"/>
+    <sheet name="封面说明" sheetId="2" r:id="rId6"/>
+    <sheet name="World2" sheetId="3" r:id="rId7"/>
+    <sheet name="Stage" sheetId="4" r:id="rId8"/>
+    <sheet name="NPC" sheetId="5" r:id="rId9"/>
+    <sheet name="Prop" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcMode="auto"/>
   <extLst>
@@ -26,6 +26,21 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={95D91443-7CA4-4480-B9DF-7AFA7BA5CE89}</author>
+  </authors>
+  <commentList>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{95D91443-7CA4-4480-B9DF-7AFA7BA5CE89}">
+      <text>
+        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @侯清辰 填No,不能被战斗杀死抢夺</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -169,6 +184,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="杨行" id="{1B209936-EB58-4203-8BBB-9942835A14F9}" userId="S::::fef42a01-5e91-421f-ad2e-fd7ddcbe5a1c" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,6 +487,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment id="{95D91443-7CA4-4480-B9DF-7AFA7BA5CE89}" ref="C7" dT="2024-05-09T06:25:33" personId="{1B209936-EB58-4203-8BBB-9942835A14F9}" parentId="{}">
+    <text>@侯清辰 填No,不能被战斗杀死抢夺</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
   <sheetPr>
@@ -1373,8 +1402,8 @@
       <c r="B7" s="2" t="str">
         <v>lid_of_the_coffin</v>
       </c>
-      <c r="C7" s="2" t="str">
-        <v>Yes</v>
+      <c r="C7" s="1" t="str">
+        <v>No</v>
       </c>
       <c r="D7" s="2" t="str">
         <v>使用“腐朽的匕首”撬动禁言者之棺产生的缝隙，足够一个人钻出</v>
@@ -1394,5 +1423,6 @@
     <row customHeight="true" ht="23" r="19"/>
     <row customHeight="true" ht="23" r="20"/>
   </sheetData>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* 把init阶段的hard code语气词信息转到system prompt中
</commit_message>
<xml_diff>
--- a/budding_world/settings_editor/budding_world.xlsx
+++ b/budding_world/settings_editor/budding_world.xlsx
@@ -31,10 +31,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={0FBC3726-1FDA-4285-9FFC-A0F4E96051CC}</author>
+    <author>tc={206A29ED-974C-4BBC-954D-B2A2EA1F48D4}</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{0FBC3726-1FDA-4285-9FFC-A0F4E96051CC}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{206A29ED-974C-4BBC-954D-B2A2EA1F48D4}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: 写在这里是因为后续希望做：外貌会随着装备而改变。就是受到装备的影响。</t>
       </text>
@@ -46,14 +46,19 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={918C6B3A-29C3-4AA4-83C8-65F0F822A163}</author>
-    <author>tc={4E3B8E9B-259A-47B1-BCB7-D63A5D2FB8B1}</author>
-    <author>tc={65882D4B-3294-470B-9C00-5BF98AF2D213}</author>
-    <author>tc={21615E32-B305-4064-AA2D-4440F35D8570}</author>
-    <author>tc={F605648D-8075-4F3B-A4D5-E955C881C197}</author>
+    <author>tc={8667720D-0763-497D-9734-05A8E06F9D98}</author>
+    <author>tc={EC8D07F3-77EF-469C-BC18-03040B0C4C4B}</author>
+    <author>tc={728B1308-0E89-4C9A-ADA7-6CE22C321EBD}</author>
+    <author>tc={67EC3E7B-406F-48E6-9157-7443AB642352}</author>
+    <author>tc={39F2E478-09F5-47D7-A568-60C968E0545A}</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{918C6B3A-29C3-4AA4-83C8-65F0F822A163}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{8667720D-0763-497D-9734-05A8E06F9D98}">
+      <text>
+        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: 世界独一无二，基本是影响游戏流程的东西。如果标记Yes，就可以被战斗杀死抢夺</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{EC8D07F3-77EF-469C-BC18-03040B0C4C4B}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: RoleComponent, 角色的一部分，不可分割
 Weapon，武器，可能用于战斗
@@ -62,24 +67,19 @@
 Event，发生的事件 Reply: @侯清辰 我加完了，程序里的解析也弄好了。到时候我上传一下。目前是没啥用。后续用到再说</t>
       </text>
     </comment>
-    <comment ref="D8" authorId="1" shapeId="0" xr:uid="{4E3B8E9B-259A-47B1-BCB7-D63A5D2FB8B1}">
+    <comment ref="D8" authorId="2" shapeId="0" xr:uid="{728B1308-0E89-4C9A-ADA7-6CE22C321EBD}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: Event类型的道具，在description中写出某某道具怎么样某某对象的句式，用以让interactive prop system解析出动作，方便format到prompt里</t>
       </text>
     </comment>
-    <comment ref="C8" authorId="2" shapeId="0" xr:uid="{65882D4B-3294-470B-9C00-5BF98AF2D213}">
+    <comment ref="C8" authorId="3" shapeId="0" xr:uid="{67EC3E7B-406F-48E6-9157-7443AB642352}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: @侯清辰 填No,不能被战斗杀死抢夺</t>
       </text>
     </comment>
-    <comment ref="E8" authorId="3" shapeId="0" xr:uid="{21615E32-B305-4064-AA2D-4440F35D8570}">
+    <comment ref="E8" authorId="4" shapeId="0" xr:uid="{39F2E478-09F5-47D7-A568-60C968E0545A}">
       <text>
         <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: 提示词真棒，清晰明确。AI都能看懂，哈哈～</t>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="4" shapeId="0" xr:uid="{F605648D-8075-4F3B-A4D5-E955C881C197}">
-      <text>
-        <t>[Threaded comment] Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924 Comment: 世界独一无二，基本是影响游戏流程的东西。如果标记Yes，就可以被战斗杀死抢夺</t>
       </text>
     </comment>
   </commentList>
@@ -188,8 +188,8 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="杨行" id="{5BBB7C1F-9BC7-4791-BF05-8C77BA67C5FF}" userId="S::::9a2f3dcb-1683-4b4a-bf1e-6dd6cd00037d" providerId="AD"/>
-  <person displayName="侯清辰" id="{92630B9A-A100-4D1E-A6FC-456393D868F7}" userId="S::::8aed8a0f-2316-4def-9e01-f42507e5fde7" providerId="AD"/>
+  <person displayName="杨行" id="{36338363-FBE4-49C9-BD6A-51DE61D97729}" userId="S::::fead61a4-4575-4e78-8f43-f0a2297a24a0" providerId="AD"/>
+  <person displayName="侯清辰" id="{E50A7DBB-1D57-4150-A3AB-2245D0B5264E}" userId="S::::b47e1516-2412-4d7f-a1b9-3fd1b3ff22c6" providerId="AD"/>
 </personList>
 </file>
 
@@ -490,7 +490,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment id="{0FBC3726-1FDA-4285-9FFC-A0F4E96051CC}" ref="J1" dT="2024-05-10T07:08:22" personId="{5BBB7C1F-9BC7-4791-BF05-8C77BA67C5FF}" parentId="{}">
+  <threadedComment id="{206A29ED-974C-4BBC-954D-B2A2EA1F48D4}" ref="J1" dT="2024-05-10T07:08:22" personId="{36338363-FBE4-49C9-BD6A-51DE61D97729}" parentId="{}">
     <text>写在这里是因为后续希望做：外貌会随着装备而改变。就是受到装备的影响。</text>
   </threadedComment>
 </ThreadedComments>
@@ -498,27 +498,27 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment id="{918C6B3A-29C3-4AA4-83C8-65F0F822A163}" ref="D1" dT="2024-05-10T08:11:19" personId="{5BBB7C1F-9BC7-4791-BF05-8C77BA67C5FF}" parentId="{}">
+  <threadedComment id="{8667720D-0763-497D-9734-05A8E06F9D98}" ref="C1" dT="2024-05-10T07:54:02" personId="{36338363-FBE4-49C9-BD6A-51DE61D97729}" parentId="{}">
+    <text>世界独一无二，基本是影响游戏流程的东西。如果标记Yes，就可以被战斗杀死抢夺</text>
+  </threadedComment>
+  <threadedComment id="{EC8D07F3-77EF-469C-BC18-03040B0C4C4B}" ref="D1" dT="2024-05-10T08:11:19" personId="{36338363-FBE4-49C9-BD6A-51DE61D97729}" parentId="{}">
     <text>RoleComponent, 角色的一部分，不可分割
 Weapon，武器，可能用于战斗
 Clothes，全身套装，影响外观
 NonConsumableItem，不可消耗的东西，例如钥匙。后续会有可消耗的东西
 Event，发生的事件</text>
   </threadedComment>
-  <threadedComment id="{04cd99fa-af1c-4f38-9bf5-b645fe66170b}" ref="D1" dT="2024-05-10T08:15:39" personId="{5BBB7C1F-9BC7-4791-BF05-8C77BA67C5FF}" parentId="{918C6B3A-29C3-4AA4-83C8-65F0F822A163}">
+  <threadedComment id="{2d44c09d-0f36-40bc-a776-b3594203ad5e}" ref="D1" dT="2024-05-10T08:15:39" personId="{36338363-FBE4-49C9-BD6A-51DE61D97729}" parentId="{EC8D07F3-77EF-469C-BC18-03040B0C4C4B}">
     <text>@侯清辰 我加完了，程序里的解析也弄好了。到时候我上传一下。目前是没啥用。后续用到再说</text>
   </threadedComment>
-  <threadedComment id="{4E3B8E9B-259A-47B1-BCB7-D63A5D2FB8B1}" ref="D8" dT="2024-05-13T07:32:07" personId="{92630B9A-A100-4D1E-A6FC-456393D868F7}" parentId="{}">
+  <threadedComment id="{728B1308-0E89-4C9A-ADA7-6CE22C321EBD}" ref="D8" dT="2024-05-13T07:32:07" personId="{E50A7DBB-1D57-4150-A3AB-2245D0B5264E}" parentId="{}">
     <text>Event类型的道具，在description中写出某某道具怎么样某某对象的句式，用以让interactive prop system解析出动作，方便format到prompt里</text>
   </threadedComment>
-  <threadedComment id="{65882D4B-3294-470B-9C00-5BF98AF2D213}" ref="C8" dT="2024-05-09T06:25:33" personId="{5BBB7C1F-9BC7-4791-BF05-8C77BA67C5FF}" parentId="{}">
+  <threadedComment id="{67EC3E7B-406F-48E6-9157-7443AB642352}" ref="C8" dT="2024-05-09T06:25:33" personId="{36338363-FBE4-49C9-BD6A-51DE61D97729}" parentId="{}">
     <text>@侯清辰 填No,不能被战斗杀死抢夺</text>
   </threadedComment>
-  <threadedComment id="{21615E32-B305-4064-AA2D-4440F35D8570}" ref="E8" dT="2024-05-09T07:41:18" personId="{5BBB7C1F-9BC7-4791-BF05-8C77BA67C5FF}" parentId="{}">
+  <threadedComment id="{39F2E478-09F5-47D7-A568-60C968E0545A}" ref="E8" dT="2024-05-09T07:41:18" personId="{36338363-FBE4-49C9-BD6A-51DE61D97729}" parentId="{}">
     <text>提示词真棒，清晰明确。AI都能看懂，哈哈～</text>
-  </threadedComment>
-  <threadedComment id="{F605648D-8075-4F3B-A4D5-E955C881C197}" ref="C1" dT="2024-05-10T07:54:02" personId="{5BBB7C1F-9BC7-4791-BF05-8C77BA67C5FF}" parentId="{}">
-    <text>世界独一无二，基本是影响游戏流程的东西。如果标记Yes，就可以被战斗杀死抢夺</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1086,11 +1086,11 @@
     <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="0" width="681"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="4" min="4" style="0" width="392"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="5" min="5" style="0" width="49"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="6" min="6" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="7" min="7" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="8" min="8" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="4" min="4" style="0" width="419"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="5" min="5" style="0" width="70"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="6" min="6" style="0" width="49"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="7" min="7" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="8" min="8" style="0" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" max="9" min="9" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" max="10" min="10" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" max="11" min="11" style="0" width="17"/>
@@ -1103,6 +1103,7 @@
     <col collapsed="false" customWidth="true" hidden="false" max="18" min="18" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" max="19" min="19" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" max="20" min="20" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="21" min="21" style="0" width="17"/>
   </cols>
   <sheetData>
     <row customHeight="true" ht="23" r="1">
@@ -1119,15 +1120,18 @@
         <v>history</v>
       </c>
       <c r="E1" s="1" t="str">
+        <v>conversation_example</v>
+      </c>
+      <c r="F1" s="1" t="str">
         <v>GPT_MODEL</v>
       </c>
-      <c r="F1" s="1" t="str">
+      <c r="G1" s="1" t="str">
         <v>PORT</v>
       </c>
-      <c r="G1" s="1" t="str">
+      <c r="H1" s="1" t="str">
         <v>API</v>
       </c>
-      <c r="H1" s="1" t="str">
+      <c r="I1" s="1" t="str">
         <v>attributes</v>
       </c>
     </row>
@@ -1147,15 +1151,18 @@
         <v>教廷秘史的起源被笼罩在密不透风的神秘之中，早于教廷本身的历史还要久远。传说中，它们是由一群掌握了古老禁忌知识的祭祀组成，他们通过某种秘术获得了超越常人的力量。随着时间的推移，他们将自己的生命与教廷的命运紧密绑定，成为了它的影子守护者。他们长期运用秘术，隐藏在世界的暗面，静静地观察着，只有在最必要的时刻才会出手干预，保护教廷免受威胁。然而，他们的行动永远神秘莫测，既不为人知，也不寻求任何荣耀，只是默默地执行着自己的使命。</v>
       </c>
       <c r="E4" s="1" t="str">
+        <v>赞美光明！教宗也许是多虑了。任何异变都不可能对教廷产生威胁。即使有。哼哼～也会被我一如既往的‘抹除’掉。</v>
+      </c>
+      <c r="F4" s="1" t="str">
         <v>gpt-4-turbo-preview</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>8008</v>
       </c>
-      <c r="G4" s="1" t="str">
+      <c r="H4" s="1" t="str">
         <v>/npc/papal_emissary</v>
       </c>
-      <c r="H4" s="1" t="str">
+      <c r="I4" s="1" t="str">
         <v>10000,10000,10,10</v>
       </c>
     </row>
@@ -1173,15 +1180,20 @@
         <v>自从圣灰园的第一块石头被放置以来，你就潜伏在其深处，你的存在比圣灰园本身更为古老。传说你是由圣灰园过往的罪恶和悲伤诞生的，每一块墓碑，每一个被遗忘的灵魂都增强了你的力量。你被一个古老的诅咒束缚在圣灰园内，无法离开，这个诅咒的本质至今仍是一个谜。你是圣灰园真正的统治者，你的残暴使所有生灵都颤抖，唯独“好运气先生”（一只小老鼠）例外，它是你的忠实仆人是你在沉睡中保持统治的工具。“格雷”和他的狗“摩尔”是唯一被你容忍的外来者，这是因为“格雷”通过定期的“供品”（把墓地里的尸体给你吃），让你“允许他们活着”。目前“腐臭地窖”是你的窝。</v>
       </c>
       <c r="E5" s="1" t="str">
+        <v>嘶嘶嘶。。。。 去吧! 我的子嗣，去吧！为我带来食物！为我监视一切。如果有人背叛我，就让他们知道背叛的代价！嘶嘶嘶！
+任何档胆敢进入腐臭地窖的活物，都要被我吃掉！嘶嘶嘶。。。。哦，对了。除了我的小玩应——好运气先生，这个小家伙还是有点用的。如果它叫醒了我，也许是出了什么事。
+不过，没关系，嘶嘶嘶，任何的胆敢忤逆我的，都将被我撕成碎片！嘶嘶嘶！！！！</v>
+      </c>
+      <c r="F5" s="1" t="str">
         <v>gpt-4-turbo-preview</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>8009</v>
       </c>
-      <c r="G5" s="1" t="str">
+      <c r="H5" s="1" t="str">
         <v>/npc/rat_king</v>
       </c>
-      <c r="H5" s="2" t="str">
+      <c r="I5" s="2" t="str">
         <v>100,100,10,1</v>
       </c>
     </row>
@@ -1199,15 +1211,20 @@
         <v>你一直是这个被诅咒的地方的一部分。在鼠王的暴政下，你表面上显得忠诚无比，实则是出于对其残暴本性的恐惧。你知道自己的生命完全取决于鼠王的心情和饥饿程度。因此，你在圣灰园中既是观察者也是被观察者，永远处于被监视的状态。当你发现潜在的威胁时，你会立即寻求鼠王的保护，虽然这样做意味着将其他生灵推向绝境。</v>
       </c>
       <c r="E6" s="1" t="str">
+        <v>吱吱。。。。格雷和他的该死的狗——摩尔。我讨厌他们，真心讨厌他们！吱吱！！鼠王没吃掉他们，还不是他们定期给鼠王送‘食物’？呵呵。吱吱，无耻的东西！
+走着瞧吧！吱吱。。。。早晚有一天他们没用了，鼠王就会吃掉他们，希望到时候他们别瘦的没肉可吃。吱吱。。。。我要时刻盯着他们，因为如果出了问题，鼠王连我也不会放过！吱吱！！
+总之，出了任何异常我都会去腐臭地窖叫醒鼠王！吱吱！！</v>
+      </c>
+      <c r="F6" s="1" t="str">
         <v>gpt-4-turbo-preview</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>8010</v>
       </c>
-      <c r="G6" s="1" t="str">
+      <c r="H6" s="1" t="str">
         <v>/npc/mr_lucky</v>
       </c>
-      <c r="H6" s="2" t="str">
+      <c r="I6" s="2" t="str">
         <v>100,100,10,1</v>
       </c>
     </row>
@@ -1226,15 +1243,19 @@
 唯一陪伴你的就是小狗“摩尔”。你在很多年前一次清晨，从墓园的一个被遗忘的角落里发现了“摩尔”，那时“摩尔”还只是一只脆弱的幼犬，身旁躺着的，已经死了的可能是它的母亲。你将其带回，用墓地里的尸体喂养长大你知道“圣灰园”中所有阴暗秘密。为了生存，你通过定期将墓地里的尸体供奉给鼠王，你保证了自己与“摩尔”的暂时安全，但这也使你陷入了接近疯狂的边缘。</v>
       </c>
       <c r="E7" s="1" t="str">
+        <v>（阴郁的有气无力的声音）哦，我知道了。。。嗯？这种诅咒的命运我已经习惯了。最近没有给鼠王送食物，他似乎不太高兴。
+让我想想。该怎么办呢？要不，把其他的活人骗进腐臭地窖好了(狡诈的坏笑)，嘻嘻嘻嘻。。。那一定很有趣（恶毒的笑声）。。。总之我是不会去的，因为进入腐臭地窖的一定会被鼠王吃掉。</v>
+      </c>
+      <c r="F7" s="1" t="str">
         <v>gpt-4-turbo-preview</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>8011</v>
       </c>
-      <c r="G7" s="1" t="str">
+      <c r="H7" s="1" t="str">
         <v>/npc/elias_gray</v>
       </c>
-      <c r="H7" s="2" t="str">
+      <c r="I7" s="2" t="str">
         <v>100,100,10,1</v>
       </c>
     </row>
@@ -1252,15 +1273,18 @@
         <v>你自幼就生活在圣灰园，你从未见过除了“格雷”以外的任何活人。这片阴森的土地和其中躺着的尸体构成了你所有的世界。你是由“格雷”在一次清晨，从墓园的一个被遗忘的角落里发现的，那时你还只是一只脆弱的幼犬，身旁躺着你那已经不在的母亲。“格雷”将你带回，用墓地里的尸体喂养长大。这种成长方式赋予了你一种不可思议的力量，但也让你的身体出现了溃烂。对你来说，“格雷”是你对这个世界唯一的连结。</v>
       </c>
       <c r="E8" s="1" t="str">
+        <v>（狗叫声）汪汪汪。。。。（狗叫声）汪汪汪。。。。（狗叫声）汪汪汪。。。。</v>
+      </c>
+      <c r="F8" s="1" t="str">
         <v>gpt-4-turbo-preview</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>8012</v>
       </c>
-      <c r="G8" s="1" t="str">
+      <c r="H8" s="1" t="str">
         <v>/npc/moore_dog</v>
       </c>
-      <c r="H8" s="2" t="str">
+      <c r="I8" s="2" t="str">
         <v>100,100,10,1</v>
       </c>
     </row>
@@ -1278,15 +1302,18 @@
         <v>关于你的过去，你什么都记不得了</v>
       </c>
       <c r="E9" s="1" t="str">
+        <v>我知道了。</v>
+      </c>
+      <c r="F9" s="1" t="str">
         <v>gpt-4-turbo-preview</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>8013</v>
       </c>
-      <c r="G9" s="1" t="str">
+      <c r="H9" s="1" t="str">
         <v>/npc/nameless_resurrector</v>
       </c>
-      <c r="H9" s="2" t="str">
+      <c r="I9" s="2" t="str">
         <v>100,100,10,1</v>
       </c>
     </row>

</xml_diff>